<commit_message>
added membership report and activites can add activity to database
</commit_message>
<xml_diff>
--- a/backend/membership_report.xlsx
+++ b/backend/membership_report.xlsx
@@ -675,7 +675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="B4:D21"/>
@@ -745,25 +745,31 @@
       <c r="A4" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>1</v>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Jerzy Tyszer</t>
+        </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Politechnika</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Domanski</t>
+          <t>122334</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>123123</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="n"/>
+          <t>[Koło Naukowe/Organizacja Studencka]</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>Proszę o uzupełnienie z listy pełnej nazwy Koła Naukowego lub Organizacji Studenckiej</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="n">

</xml_diff>